<commit_message>
MS549 Assignment 2 - Video and ZIP
* Added .mkv video walkthrough of the assignment.
* Added .zip containing documentation.
* Added .zip containing performance results.
</commit_message>
<xml_diff>
--- a/MS549/Assignment2_LinkedList/PerformanceResults.xlsx
+++ b/MS549/Assignment2_LinkedList/PerformanceResults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\otaku\Documents\UAT School Projects\MS549\Assignment2_LinkedList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65FA317-4FF7-4EFC-BC5B-BA9571A4C08C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C28ED4-D100-4933-A01A-4CF76FF05970}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CB042D6E-24D6-4C26-BC19-F5ACD6AD2425}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CB042D6E-24D6-4C26-BC19-F5ACD6AD2425}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -287,15 +287,6 @@
   </cellStyleXfs>
   <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -303,6 +294,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="2" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="8" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="9" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -330,15 +339,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="8" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="9" xfId="2" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent3" xfId="2" builtinId="38"/>
@@ -1203,13 +1203,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>8.14</c:v>
+                  <c:v>27.21</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>233.13</c:v>
+                  <c:v>1171.3699999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3982.69</c:v>
+                  <c:v>116726.36</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3118,7 +3118,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3127,156 +3127,156 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4"/>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="2"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="19"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
+      <c r="A3" s="6">
         <v>10</v>
       </c>
-      <c r="B3" s="20">
+      <c r="B3" s="8">
         <v>16.11</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="9">
         <v>8.4499999999999993</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D3" s="10">
         <v>5.37</v>
       </c>
-      <c r="E3" s="20">
+      <c r="E3" s="8">
         <v>32</v>
       </c>
-      <c r="F3" s="21">
-        <v>8.14</v>
-      </c>
-      <c r="G3" s="22">
+      <c r="F3" s="9">
+        <v>27.21</v>
+      </c>
+      <c r="G3" s="10">
         <v>52.27</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="2">
         <v>100</v>
       </c>
-      <c r="B4" s="23">
+      <c r="B4" s="11">
         <v>177.67</v>
       </c>
-      <c r="C4" s="24">
+      <c r="C4" s="12">
         <v>119.45</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="13">
         <v>23.28</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="11">
         <v>3142.26</v>
       </c>
-      <c r="F4" s="24">
-        <v>233.13</v>
-      </c>
-      <c r="G4" s="25">
+      <c r="F4" s="12">
+        <v>1171.3699999999999</v>
+      </c>
+      <c r="G4" s="13">
         <v>1569.3</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+      <c r="A5" s="6">
         <v>1000</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5" s="8">
         <v>1431.22</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="9">
         <v>523.21</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="10">
         <v>274.25</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E5" s="8">
         <v>271867.87</v>
       </c>
-      <c r="F5" s="21">
-        <v>3982.69</v>
-      </c>
-      <c r="G5" s="22">
+      <c r="F5" s="9">
+        <v>116726.36</v>
+      </c>
+      <c r="G5" s="10">
         <v>149470.73000000001</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="2">
         <v>10000</v>
       </c>
-      <c r="B6" s="23">
+      <c r="B6" s="11">
         <v>11013.89</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C6" s="12">
         <v>4833.1400000000003</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="13">
         <v>2475.1</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="16"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="25"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10">
+      <c r="A7" s="7">
         <v>100000</v>
       </c>
-      <c r="B7" s="26">
+      <c r="B7" s="14">
         <v>136649.5</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C7" s="15">
         <v>94022.87</v>
       </c>
-      <c r="D7" s="28">
+      <c r="D7" s="16">
         <v>20616.21</v>
       </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="19"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="28"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="13"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>